<commit_message>
modified:   Band2MaxPowerInput1_FrequencySweepRanges.xlsx 	modified:   Band2MinPowerInput1_FrequencySweepRanges.xlsx 	modified:   FSW_test_5ranges.py
</commit_message>
<xml_diff>
--- a/Minpowerinputfile.xlsx
+++ b/Minpowerinputfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB54FB4-AF64-40F1-B3A0-780021D83F77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56DF5E5-882E-44B9-B0DC-397B304925A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="600" windowWidth="25500" windowHeight="14265" activeTab="2" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F21EF5-0615-4121-83E8-517FC8180B1A}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8596D56-7C71-4D72-A666-9CAEA981CBE7}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>